<commit_message>
Melhorias na automação e categorização
</commit_message>
<xml_diff>
--- a/Analíse_relaçao_economiasEgastos.xlsx
+++ b/Analíse_relaçao_economiasEgastos.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAMSUNG\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\OneDrive\Área de Trabalho\Cointech\IA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D34947-BADE-4F41-AF0E-7345B97941CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21A9F19-24E7-4139-B4FB-2DA81DDCE4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1CAA09A8-590D-4065-95D4-4E380225DD42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CAA09A8-590D-4065-95D4-4E380225DD42}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Usuário</t>
   </si>
@@ -69,6 +70,9 @@
   </si>
   <si>
     <t>Bicos</t>
+  </si>
+  <si>
+    <t>Poupança</t>
   </si>
 </sst>
 </file>
@@ -466,15 +470,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD84ECFB-3D90-4DF8-96C4-76C449649BB5}">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="L101" sqref="L101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,8 +512,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -543,8 +550,12 @@
       <c r="K2">
         <v>300</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <f>IFERROR(SUM(J2:K2) - SUM(B2:I2), 0)</f>
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -578,8 +589,12 @@
       <c r="K3">
         <v>600</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <f>IFERROR(SUM(J3:K3) - SUM(B3:I3), 0)</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -613,8 +628,12 @@
       <c r="K4">
         <v>900</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <f>IFERROR(SUM(J4:K4) - SUM(B4:I4), 0)</f>
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -648,8 +667,12 @@
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <f>IFERROR(SUM(J5:K5) - SUM(B5:I5), 0)</f>
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -683,8 +706,12 @@
       <c r="K6">
         <v>300</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <f>IFERROR(SUM(J6:K6) - SUM(B6:I6), 0)</f>
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -718,8 +745,12 @@
       <c r="K7">
         <v>600</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <f>IFERROR(SUM(J7:K7) - SUM(B7:I7), 0)</f>
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -753,8 +784,12 @@
       <c r="K8">
         <v>900</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <f>IFERROR(SUM(J8:K8) - SUM(B8:I8), 0)</f>
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -788,8 +823,12 @@
       <c r="K9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <f>IFERROR(SUM(J9:K9) - SUM(B9:I9), 0)</f>
+        <v>2740</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -823,8 +862,12 @@
       <c r="K10">
         <v>300</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <f>IFERROR(SUM(J10:K10) - SUM(B10:I10), 0)</f>
+        <v>3210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -858,8 +901,12 @@
       <c r="K11">
         <v>600</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <f>IFERROR(SUM(J11:K11) - SUM(B11:I11), 0)</f>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -893,8 +940,12 @@
       <c r="K12">
         <v>900</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <f>IFERROR(SUM(J12:K12) - SUM(B12:I12), 0)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -928,8 +979,12 @@
       <c r="K13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <f>IFERROR(SUM(J13:K13) - SUM(B13:I13), 0)</f>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -963,8 +1018,12 @@
       <c r="K14">
         <v>300</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <f>IFERROR(SUM(J14:K14) - SUM(B14:I14), 0)</f>
+        <v>860</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -998,8 +1057,12 @@
       <c r="K15">
         <v>600</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <f>IFERROR(SUM(J15:K15) - SUM(B15:I15), 0)</f>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1033,8 +1096,12 @@
       <c r="K16">
         <v>900</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <f>IFERROR(SUM(J16:K16) - SUM(B16:I16), 0)</f>
+        <v>3170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1068,8 +1135,12 @@
       <c r="K17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <f>IFERROR(SUM(J17:K17) - SUM(B17:I17), 0)</f>
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1103,8 +1174,12 @@
       <c r="K18">
         <v>300</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <f>IFERROR(SUM(J18:K18) - SUM(B18:I18), 0)</f>
+        <v>2990</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1138,8 +1213,12 @@
       <c r="K19">
         <v>600</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <f>IFERROR(SUM(J19:K19) - SUM(B19:I19), 0)</f>
+        <v>3580</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1173,8 +1252,12 @@
       <c r="K20">
         <v>900</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <f>IFERROR(SUM(J20:K20) - SUM(B20:I20), 0)</f>
+        <v>4050</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1208,8 +1291,12 @@
       <c r="K21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <f>IFERROR(SUM(J21:K21) - SUM(B21:I21), 0)</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1243,8 +1330,12 @@
       <c r="K22">
         <v>300</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22">
+        <f>IFERROR(SUM(J22:K22) - SUM(B22:I22), 0)</f>
+        <v>710</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1278,8 +1369,12 @@
       <c r="K23">
         <v>600</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <f>IFERROR(SUM(J23:K23) - SUM(B23:I23), 0)</f>
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1313,8 +1408,12 @@
       <c r="K24">
         <v>900</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24">
+        <f>IFERROR(SUM(J24:K24) - SUM(B24:I24), 0)</f>
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1348,8 +1447,12 @@
       <c r="K25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <f>IFERROR(SUM(J25:K25) - SUM(B25:I25), 0)</f>
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1383,8 +1486,12 @@
       <c r="K26">
         <v>300</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L26">
+        <f>IFERROR(SUM(J26:K26) - SUM(B26:I26), 0)</f>
+        <v>2140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1418,8 +1525,12 @@
       <c r="K27">
         <v>600</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L27">
+        <f>IFERROR(SUM(J27:K27) - SUM(B27:I27), 0)</f>
+        <v>2610</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1453,8 +1564,12 @@
       <c r="K28">
         <v>900</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28">
+        <f>IFERROR(SUM(J28:K28) - SUM(B28:I28), 0)</f>
+        <v>3080</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1488,8 +1603,12 @@
       <c r="K29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L29">
+        <f>IFERROR(SUM(J29:K29) - SUM(B29:I29), 0)</f>
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1523,8 +1642,12 @@
       <c r="K30">
         <v>300</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30">
+        <f>IFERROR(SUM(J30:K30) - SUM(B30:I30), 0)</f>
+        <v>2890</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1558,8 +1681,12 @@
       <c r="K31">
         <v>600</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L31">
+        <f>IFERROR(SUM(J31:K31) - SUM(B31:I31), 0)</f>
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1593,8 +1720,12 @@
       <c r="K32">
         <v>900</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L32">
+        <f>IFERROR(SUM(J32:K32) - SUM(B32:I32), 0)</f>
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1628,8 +1759,12 @@
       <c r="K33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <f>IFERROR(SUM(J33:K33) - SUM(B33:I33), 0)</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1663,8 +1798,12 @@
       <c r="K34">
         <v>300</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L34">
+        <f>IFERROR(SUM(J34:K34) - SUM(B34:I34), 0)</f>
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1698,8 +1837,12 @@
       <c r="K35">
         <v>600</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L35">
+        <f>IFERROR(SUM(J35:K35) - SUM(B35:I35), 0)</f>
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1733,8 +1876,12 @@
       <c r="K36">
         <v>900</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L36">
+        <f>IFERROR(SUM(J36:K36) - SUM(B36:I36), 0)</f>
+        <v>2930</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1768,8 +1915,12 @@
       <c r="K37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L37">
+        <f>IFERROR(SUM(J37:K37) - SUM(B37:I37), 0)</f>
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1803,8 +1954,12 @@
       <c r="K38">
         <v>300</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L38">
+        <f>IFERROR(SUM(J38:K38) - SUM(B38:I38), 0)</f>
+        <v>2790</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1838,8 +1993,12 @@
       <c r="K39">
         <v>600</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L39">
+        <f>IFERROR(SUM(J39:K39) - SUM(B39:I39), 0)</f>
+        <v>3260</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1873,8 +2032,12 @@
       <c r="K40">
         <v>900</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L40">
+        <f>IFERROR(SUM(J40:K40) - SUM(B40:I40), 0)</f>
+        <v>3730</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1908,8 +2071,12 @@
       <c r="K41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L41">
+        <f>IFERROR(SUM(J41:K41) - SUM(B41:I41), 0)</f>
+        <v>-70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1943,8 +2110,12 @@
       <c r="K42">
         <v>300</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L42">
+        <f>IFERROR(SUM(J42:K42) - SUM(B42:I42), 0)</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1978,8 +2149,12 @@
       <c r="K43">
         <v>600</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L43">
+        <f>IFERROR(SUM(J43:K43) - SUM(B43:I43), 0)</f>
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2013,8 +2188,12 @@
       <c r="K44">
         <v>900</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L44">
+        <f>IFERROR(SUM(J44:K44) - SUM(B44:I44), 0)</f>
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2048,8 +2227,12 @@
       <c r="K45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L45">
+        <f>IFERROR(SUM(J45:K45) - SUM(B45:I45), 0)</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2083,8 +2266,12 @@
       <c r="K46">
         <v>300</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L46">
+        <f>IFERROR(SUM(J46:K46) - SUM(B46:I46), 0)</f>
+        <v>2570</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2118,8 +2305,12 @@
       <c r="K47">
         <v>600</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L47">
+        <f>IFERROR(SUM(J47:K47) - SUM(B47:I47), 0)</f>
+        <v>3040</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2153,8 +2344,12 @@
       <c r="K48">
         <v>900</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L48">
+        <f>IFERROR(SUM(J48:K48) - SUM(B48:I48), 0)</f>
+        <v>3510</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2188,8 +2383,12 @@
       <c r="K49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L49">
+        <f>IFERROR(SUM(J49:K49) - SUM(B49:I49), 0)</f>
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2223,8 +2422,12 @@
       <c r="K50">
         <v>300</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L50">
+        <f>IFERROR(SUM(J50:K50) - SUM(B50:I50), 0)</f>
+        <v>3520</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2258,8 +2461,12 @@
       <c r="K51">
         <v>600</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L51">
+        <f>IFERROR(SUM(J51:K51) - SUM(B51:I51), 0)</f>
+        <v>840</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2293,8 +2500,12 @@
       <c r="K52">
         <v>900</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L52">
+        <f>IFERROR(SUM(J52:K52) - SUM(B52:I52), 0)</f>
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2328,8 +2539,12 @@
       <c r="K53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L53">
+        <f>IFERROR(SUM(J53:K53) - SUM(B53:I53), 0)</f>
+        <v>580</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2363,8 +2578,12 @@
       <c r="K54">
         <v>300</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L54">
+        <f>IFERROR(SUM(J54:K54) - SUM(B54:I54), 0)</f>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2398,8 +2617,12 @@
       <c r="K55">
         <v>600</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L55">
+        <f>IFERROR(SUM(J55:K55) - SUM(B55:I55), 0)</f>
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2433,8 +2656,12 @@
       <c r="K56">
         <v>900</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L56">
+        <f>IFERROR(SUM(J56:K56) - SUM(B56:I56), 0)</f>
+        <v>2660</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2468,8 +2695,12 @@
       <c r="K57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L57">
+        <f>IFERROR(SUM(J57:K57) - SUM(B57:I57), 0)</f>
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2503,8 +2734,12 @@
       <c r="K58">
         <v>300</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L58">
+        <f>IFERROR(SUM(J58:K58) - SUM(B58:I58), 0)</f>
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2538,8 +2773,12 @@
       <c r="K59">
         <v>600</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L59">
+        <f>IFERROR(SUM(J59:K59) - SUM(B59:I59), 0)</f>
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2573,8 +2812,12 @@
       <c r="K60">
         <v>900</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L60">
+        <f>IFERROR(SUM(J60:K60) - SUM(B60:I60), 0)</f>
+        <v>3490</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2608,8 +2851,12 @@
       <c r="K61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L61">
+        <f>IFERROR(SUM(J61:K61) - SUM(B61:I61), 0)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2643,8 +2890,12 @@
       <c r="K62">
         <v>300</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L62">
+        <f>IFERROR(SUM(J62:K62) - SUM(B62:I62), 0)</f>
+        <v>950</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2678,8 +2929,12 @@
       <c r="K63">
         <v>600</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L63">
+        <f>IFERROR(SUM(J63:K63) - SUM(B63:I63), 0)</f>
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2713,8 +2968,12 @@
       <c r="K64">
         <v>900</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L64">
+        <f>IFERROR(SUM(J64:K64) - SUM(B64:I64), 0)</f>
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2748,8 +3007,12 @@
       <c r="K65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L65">
+        <f>IFERROR(SUM(J65:K65) - SUM(B65:I65), 0)</f>
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2783,8 +3046,12 @@
       <c r="K66">
         <v>300</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L66">
+        <f>IFERROR(SUM(J66:K66) - SUM(B66:I66), 0)</f>
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2818,8 +3085,12 @@
       <c r="K67">
         <v>600</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L67">
+        <f>IFERROR(SUM(J67:K67) - SUM(B67:I67), 0)</f>
+        <v>2920</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2853,8 +3124,12 @@
       <c r="K68">
         <v>900</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L68">
+        <f>IFERROR(SUM(J68:K68) - SUM(B68:I68), 0)</f>
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2888,8 +3163,12 @@
       <c r="K69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L69">
+        <f>IFERROR(SUM(J69:K69) - SUM(B69:I69), 0)</f>
+        <v>2660</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2923,8 +3202,12 @@
       <c r="K70">
         <v>300</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L70">
+        <f>IFERROR(SUM(J70:K70) - SUM(B70:I70), 0)</f>
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2958,8 +3241,12 @@
       <c r="K71">
         <v>600</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L71">
+        <f>IFERROR(SUM(J71:K71) - SUM(B71:I71), 0)</f>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2993,8 +3280,12 @@
       <c r="K72">
         <v>900</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L72">
+        <f>IFERROR(SUM(J72:K72) - SUM(B72:I72), 0)</f>
+        <v>990</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3028,8 +3319,12 @@
       <c r="K73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L73">
+        <f>IFERROR(SUM(J73:K73) - SUM(B73:I73), 0)</f>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3063,8 +3358,12 @@
       <c r="K74">
         <v>300</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L74">
+        <f>IFERROR(SUM(J74:K74) - SUM(B74:I74), 0)</f>
+        <v>930</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3098,8 +3397,12 @@
       <c r="K75">
         <v>600</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L75">
+        <f>IFERROR(SUM(J75:K75) - SUM(B75:I75), 0)</f>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3133,8 +3436,12 @@
       <c r="K76">
         <v>900</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L76">
+        <f>IFERROR(SUM(J76:K76) - SUM(B76:I76), 0)</f>
+        <v>3170</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3168,8 +3475,12 @@
       <c r="K77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L77">
+        <f>IFERROR(SUM(J77:K77) - SUM(B77:I77), 0)</f>
+        <v>2440</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3203,8 +3514,12 @@
       <c r="K78">
         <v>300</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L78">
+        <f>IFERROR(SUM(J78:K78) - SUM(B78:I78), 0)</f>
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3238,8 +3553,12 @@
       <c r="K79">
         <v>600</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L79">
+        <f>IFERROR(SUM(J79:K79) - SUM(B79:I79), 0)</f>
+        <v>3570</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3273,8 +3592,12 @@
       <c r="K80">
         <v>900</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L80">
+        <f>IFERROR(SUM(J80:K80) - SUM(B80:I80), 0)</f>
+        <v>4040</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3308,8 +3631,12 @@
       <c r="K81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L81">
+        <f>IFERROR(SUM(J81:K81) - SUM(B81:I81), 0)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3343,8 +3670,12 @@
       <c r="K82">
         <v>300</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L82">
+        <f>IFERROR(SUM(J82:K82) - SUM(B82:I82), 0)</f>
+        <v>710</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3378,8 +3709,12 @@
       <c r="K83">
         <v>600</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L83">
+        <f>IFERROR(SUM(J83:K83) - SUM(B83:I83), 0)</f>
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3413,8 +3748,12 @@
       <c r="K84">
         <v>900</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L84">
+        <f>IFERROR(SUM(J84:K84) - SUM(B84:I84), 0)</f>
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3448,8 +3787,12 @@
       <c r="K85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L85">
+        <f>IFERROR(SUM(J85:K85) - SUM(B85:I85), 0)</f>
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3483,8 +3826,12 @@
       <c r="K86">
         <v>300</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L86">
+        <f>IFERROR(SUM(J86:K86) - SUM(B86:I86), 0)</f>
+        <v>2130</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3518,8 +3865,12 @@
       <c r="K87">
         <v>600</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L87">
+        <f>IFERROR(SUM(J87:K87) - SUM(B87:I87), 0)</f>
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3553,8 +3904,12 @@
       <c r="K88">
         <v>900</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L88">
+        <f>IFERROR(SUM(J88:K88) - SUM(B88:I88), 0)</f>
+        <v>3070</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3588,8 +3943,12 @@
       <c r="K89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L89">
+        <f>IFERROR(SUM(J89:K89) - SUM(B89:I89), 0)</f>
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3623,8 +3982,12 @@
       <c r="K90">
         <v>300</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L90">
+        <f>IFERROR(SUM(J90:K90) - SUM(B90:I90), 0)</f>
+        <v>2890</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3658,8 +4021,12 @@
       <c r="K91">
         <v>600</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L91">
+        <f>IFERROR(SUM(J91:K91) - SUM(B91:I91), 0)</f>
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3693,8 +4060,12 @@
       <c r="K92">
         <v>900</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L92">
+        <f>IFERROR(SUM(J92:K92) - SUM(B92:I92), 0)</f>
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3728,8 +4099,12 @@
       <c r="K93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L93">
+        <f>IFERROR(SUM(J93:K93) - SUM(B93:I93), 0)</f>
+        <v>890</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3763,8 +4138,12 @@
       <c r="K94">
         <v>300</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L94">
+        <f>IFERROR(SUM(J94:K94) - SUM(B94:I94), 0)</f>
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3798,8 +4177,12 @@
       <c r="K95">
         <v>600</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L95">
+        <f>IFERROR(SUM(J95:K95) - SUM(B95:I95), 0)</f>
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3833,8 +4216,12 @@
       <c r="K96">
         <v>900</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L96">
+        <f>IFERROR(SUM(J96:K96) - SUM(B96:I96), 0)</f>
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3868,8 +4255,12 @@
       <c r="K97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L97">
+        <f>IFERROR(SUM(J97:K97) - SUM(B97:I97), 0)</f>
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3903,8 +4294,12 @@
       <c r="K98">
         <v>300</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L98">
+        <f>IFERROR(SUM(J98:K98) - SUM(B98:I98), 0)</f>
+        <v>2790</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3938,8 +4333,12 @@
       <c r="K99">
         <v>600</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L99">
+        <f>IFERROR(SUM(J99:K99) - SUM(B99:I99), 0)</f>
+        <v>3330</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3973,8 +4372,12 @@
       <c r="K100">
         <v>900</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L100">
+        <f>IFERROR(SUM(J100:K100) - SUM(B100:I100), 0)</f>
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4007,6 +4410,10 @@
       </c>
       <c r="K101">
         <v>0</v>
+      </c>
+      <c r="L101">
+        <f>IFERROR(SUM(J101:K101) - SUM(B101:I101), 0)</f>
+        <v>-80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>